<commit_message>
agregados graficos de V y So4
</commit_message>
<xml_diff>
--- a/BA_events_testMnew2.xlsx
+++ b/BA_events_testMnew2.xlsx
@@ -126,7 +126,7 @@
     <t xml:space="preserve">Mesopotamia</t>
   </si>
   <si>
-    <t xml:space="preserve">MES (ARG)</t>
+    <t xml:space="preserve">MES</t>
   </si>
   <si>
     <t xml:space="preserve">DN</t>
@@ -177,7 +177,7 @@
     <t xml:space="preserve">Bs. As.</t>
   </si>
   <si>
-    <t xml:space="preserve">BA (ARG)</t>
+    <t xml:space="preserve">BA</t>
   </si>
   <si>
     <t xml:space="preserve">SL</t>
@@ -760,13 +760,13 @@
   </sheetPr>
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="B56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I92" activeCellId="0" sqref="I92"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="M33" activeCellId="0" sqref="M33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.83203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="15.14"/>
@@ -9177,7 +9177,7 @@
       <selection pane="bottomRight" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.83203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="2" style="0" width="10.86"/>

</xml_diff>